<commit_message>
added demo trial balance
</commit_message>
<xml_diff>
--- a/xlwings_project/enriched_template_balance_sheet.xlsx
+++ b/xlwings_project/enriched_template_balance_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Fosa/PythonProjects/git_tree/auditing_automation/xlwings_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1467DE1B-47CA-704E-8B42-A83C2821520E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726995A1-AE2E-0E4C-A36A-6F30372275AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320" xr2:uid="{6D501CA2-B23A-2B48-B2C2-E8CE2BD33026}"/>
+    <workbookView xWindow="25600" yWindow="-10040" windowWidth="51200" windowHeight="28800" xr2:uid="{6D501CA2-B23A-2B48-B2C2-E8CE2BD33026}"/>
   </bookViews>
   <sheets>
     <sheet name="Trial Balance" sheetId="4" r:id="rId1"/>
@@ -501,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7860D17A-7DEB-B94D-9AD8-7E69AEA8120E}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -578,7 +578,7 @@
         <v>8</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>